<commit_message>
Closeerr than we've ever been
</commit_message>
<xml_diff>
--- a/Super Powered/Data/Success Analysis.xlsx
+++ b/Super Powered/Data/Success Analysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FLL\repo\Super Powered\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F4A3D4-EDFC-4D32-8338-2E61979C3E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA841A-A021-45F3-BFB6-AE803C294E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{3C495B11-8F86-4B74-B5DE-F7306E2E0B1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{3C495B11-8F86-4B74-B5DE-F7306E2E0B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Full Run" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="18">
   <si>
     <t>Score</t>
   </si>
@@ -83,6 +84,15 @@
   <si>
     <t>Success Rate</t>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
 </sst>
 </file>
 
@@ -117,10 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,9 +157,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}" name="Table1" displayName="Table1" ref="A1:G150" totalsRowShown="0">
-  <autoFilter ref="A1:G150" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}" name="Table1" displayName="Table1" ref="A1:H150" totalsRowShown="0">
+  <autoFilter ref="A1:H150" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BF74B0B6-E334-4636-978E-7051EB4E0E64}" name="Trial"/>
     <tableColumn id="6" xr3:uid="{A741DFB3-5075-44B7-8804-88C9204AD3A0}" name="Run"/>
     <tableColumn id="2" xr3:uid="{B1ED5BF7-12AB-4862-A43A-F24651F2C2DE}" name="Score"/>
@@ -158,6 +169,7 @@
     <tableColumn id="7" xr3:uid="{DBB3BF7F-BF59-4269-BBD9-CA081A15D5EC}" name="Success Rate" dataDxfId="1">
       <calculatedColumnFormula>IF(ISERROR((Table1[[#This Row],[Score]]/Table1[[#This Row],[Max]]) +(Table1[[#This Row],[NSO Met]]/Table1[[#This Row],[NSO Goal]]))/2, Table1[[#This Row],[Score]]/Table1[[#This Row],[Max]], ((Table1[[#This Row],[Score]]/Table1[[#This Row],[Max]]) +(Table1[[#This Row],[NSO Met]]/Table1[[#This Row],[NSO Goal]]))/2)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{9C4DE3C3-069D-4CBF-87BF-133698B30A42}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -444,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A46FB3-1908-4E31-8006-A098B5EDCE82}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -456,9 +468,10 @@
     <col min="2" max="2" width="10.875" customWidth="1"/>
     <col min="4" max="5" width="10.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -480,8 +493,11 @@
       <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -505,7 +521,7 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(Table1[[#This Row],[Run]]=B2, A2+1, 1)</f>
         <v>2</v>
@@ -530,7 +546,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>IF(Table1[[#This Row],[Run]]=B3, A3+1, 1)</f>
         <v>3</v>
@@ -555,7 +571,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>IF(Table1[[#This Row],[Run]]=B4, A4+1, 1)</f>
         <v>4</v>
@@ -580,7 +596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>IF(Table1[[#This Row],[Run]]=B5, A5+1, 1)</f>
         <v>5</v>
@@ -605,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>IF(Table1[[#This Row],[Run]]=B6, A6+1, 1)</f>
         <v>6</v>
@@ -630,7 +646,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>IF(Table1[[#This Row],[Run]]=B7, A7+1, 1)</f>
         <v>7</v>
@@ -655,7 +671,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>IF(Table1[[#This Row],[Run]]=B8, A8+1, 1)</f>
         <v>8</v>
@@ -680,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>IF(Table1[[#This Row],[Run]]=B9, A9+1, 1)</f>
         <v>9</v>
@@ -705,7 +721,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>IF(Table1[[#This Row],[Run]]=B10, A10+1, 1)</f>
         <v>10</v>
@@ -730,7 +746,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>IF(Table1[[#This Row],[Run]]=B11, A11+1, 1)</f>
         <v>11</v>
@@ -755,7 +771,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>IF(Table1[[#This Row],[Run]]=B12, A12+1, 1)</f>
         <v>12</v>
@@ -780,7 +796,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>IF(Table1[[#This Row],[Run]]=B13, A13+1, 1)</f>
         <v>13</v>
@@ -805,7 +821,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>IF(Table1[[#This Row],[Run]]=B14, A14+1, 1)</f>
         <v>14</v>
@@ -830,7 +846,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>IF(Table1[[#This Row],[Run]]=B15, A15+1, 1)</f>
         <v>15</v>
@@ -3911,7 +3927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0249229-1DE6-4127-8B6B-6B83AFD04217}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
@@ -4823,4 +4839,74 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E476FCB0-2EF6-4003-8656-30B369C26D3E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.10833333333333334</v>
+      </c>
+      <c r="C2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.1125</v>
+      </c>
+      <c r="C3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C4">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="C5">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hola, muy mal :(
</commit_message>
<xml_diff>
--- a/Super Powered/Data/Success Analysis.xlsx
+++ b/Super Powered/Data/Success Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FLL\repo\Super Powered\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA841A-A021-45F3-BFB6-AE803C294E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D6252A-BD4E-437D-BDEA-27C7CB39FCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{3C495B11-8F86-4B74-B5DE-F7306E2E0B1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{3C495B11-8F86-4B74-B5DE-F7306E2E0B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="17">
   <si>
     <t>Score</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Points</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -157,9 +154,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}" name="Table1" displayName="Table1" ref="A1:H150" totalsRowShown="0">
-  <autoFilter ref="A1:H150" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}" name="Table1" displayName="Table1" ref="A1:G150" totalsRowShown="0">
+  <autoFilter ref="A1:G150" xr:uid="{BF35B27C-1545-4632-BE72-18A5BDAD030B}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{BF74B0B6-E334-4636-978E-7051EB4E0E64}" name="Trial"/>
     <tableColumn id="6" xr3:uid="{A741DFB3-5075-44B7-8804-88C9204AD3A0}" name="Run"/>
     <tableColumn id="2" xr3:uid="{B1ED5BF7-12AB-4862-A43A-F24651F2C2DE}" name="Score"/>
@@ -169,7 +166,6 @@
     <tableColumn id="7" xr3:uid="{DBB3BF7F-BF59-4269-BBD9-CA081A15D5EC}" name="Success Rate" dataDxfId="1">
       <calculatedColumnFormula>IF(ISERROR((Table1[[#This Row],[Score]]/Table1[[#This Row],[Max]]) +(Table1[[#This Row],[NSO Met]]/Table1[[#This Row],[NSO Goal]]))/2, Table1[[#This Row],[Score]]/Table1[[#This Row],[Max]], ((Table1[[#This Row],[Score]]/Table1[[#This Row],[Max]]) +(Table1[[#This Row],[NSO Met]]/Table1[[#This Row],[NSO Goal]]))/2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9C4DE3C3-069D-4CBF-87BF-133698B30A42}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -456,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A46FB3-1908-4E31-8006-A098B5EDCE82}">
-  <dimension ref="A1:H150"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -471,7 +467,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -493,11 +489,8 @@
       <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -521,7 +514,7 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(Table1[[#This Row],[Run]]=B2, A2+1, 1)</f>
         <v>2</v>
@@ -546,7 +539,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>IF(Table1[[#This Row],[Run]]=B3, A3+1, 1)</f>
         <v>3</v>
@@ -571,7 +564,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>IF(Table1[[#This Row],[Run]]=B4, A4+1, 1)</f>
         <v>4</v>
@@ -596,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>IF(Table1[[#This Row],[Run]]=B5, A5+1, 1)</f>
         <v>5</v>
@@ -621,7 +614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>IF(Table1[[#This Row],[Run]]=B6, A6+1, 1)</f>
         <v>6</v>
@@ -646,7 +639,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>IF(Table1[[#This Row],[Run]]=B7, A7+1, 1)</f>
         <v>7</v>
@@ -671,7 +664,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>IF(Table1[[#This Row],[Run]]=B8, A8+1, 1)</f>
         <v>8</v>
@@ -696,7 +689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>IF(Table1[[#This Row],[Run]]=B9, A9+1, 1)</f>
         <v>9</v>
@@ -721,7 +714,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>IF(Table1[[#This Row],[Run]]=B10, A10+1, 1)</f>
         <v>10</v>
@@ -746,7 +739,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>IF(Table1[[#This Row],[Run]]=B11, A11+1, 1)</f>
         <v>11</v>
@@ -771,7 +764,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>IF(Table1[[#This Row],[Run]]=B12, A12+1, 1)</f>
         <v>12</v>
@@ -796,7 +789,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>IF(Table1[[#This Row],[Run]]=B13, A13+1, 1)</f>
         <v>13</v>
@@ -821,7 +814,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>IF(Table1[[#This Row],[Run]]=B14, A14+1, 1)</f>
         <v>14</v>
@@ -846,7 +839,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>IF(Table1[[#This Row],[Run]]=B15, A15+1, 1)</f>
         <v>15</v>
@@ -3927,8 +3920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0249229-1DE6-4127-8B6B-6B83AFD04217}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4843,10 +4836,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E476FCB0-2EF6-4003-8656-30B369C26D3E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4906,6 +4899,39 @@
         <v>295</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="C6">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.10277777777777779</v>
+      </c>
+      <c r="C7">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.10347222222222223</v>
+      </c>
+      <c r="C8">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>